<commit_message>
Actualización sol graf. CN 06 05
Actualización sol graf. CN 06 05
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion05/SolicitudGrafica_CN_06_05.xlsx
+++ b/fuentes/contenidos/grado06/guion05/SolicitudGrafica_CN_06_05.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="218">
   <si>
     <t>Fecha:</t>
   </si>
@@ -641,18 +641,12 @@
     <t>Cambiar nombres a español:    Bolus of food: Bolo alimenticio      /       Pharynx: Faringe      /     Tongue: Lengua     /     Epiglottis: Epiglotis        /        Esophagus: Esófago         /   Trachea: Tráquea     /Constiction: Contracción   /   Peristaltic wave:  Movimiento peristáltico  /    Bolus: Bolo      /                Relaxation: Relajación muscular      /      Stomach: Estómago                                        Eliminar la palabra: shortening                                                                            Incluir la palabra Esófago con las líneas en los dos dibujos inferiores,  También incluir la segunda línea que señala el estómago con e dibujo izquierdo,     añadir la palabra al dibujo de abajo izquierda:  Contracción</t>
   </si>
   <si>
-    <t>http://hispanicasaber.planetasaber.com/encyclopedia/default.asp?idreg=78380&amp;ruta=Buscador</t>
-  </si>
-  <si>
     <t>Movimientos peristálticos del esófago</t>
   </si>
   <si>
     <t>Estómago</t>
   </si>
   <si>
-    <t>El título de la imagen en la biblioteca hispánica saber es:  Esquema del estómago.  Al dar clic izq. Para guardar la imagen sae el número 000Y9U01                                                                      Borrar las siguientes palabras:  Túnica serosa     /   Tuberosidad mayor gástica  /   Curvatura mayor gástrica    /      Bulbo duodenal     /      Músculo del esfínter pilórico    / curvatura menor    /     mucosa                                                                                                                                                                             Dejar el resto de nombres.</t>
-  </si>
-  <si>
     <t>6° Primaria/Ciencias de la Naturaleza/Cuaderno de estudio/El aparato digestivo y el sistema excretor/el aparato digestivo.</t>
   </si>
   <si>
@@ -684,6 +678,9 @@
   </si>
   <si>
     <t>CN_06_05_REC10</t>
+  </si>
+  <si>
+    <t>Colocar nombres y señalizaciones:  Esófago   /    Cuerpo del estómago   /   Píloro   /   Cardias   /  Duodeno</t>
   </si>
 </sst>
 </file>
@@ -1936,44 +1933,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>156881</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>123265</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>2633318</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>2364441</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17178616" y="11642912"/>
-          <a:ext cx="2476437" cy="2241176"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
       <xdr:colOff>67235</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>89648</xdr:rowOff>
@@ -1992,7 +1951,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2030,7 +1989,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2039,6 +1998,44 @@
         <a:xfrm>
           <a:off x="17100176" y="17559617"/>
           <a:ext cx="1580030" cy="1587929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2342030</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2397299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17021735" y="11519647"/>
+          <a:ext cx="2342030" cy="2397299"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2962,7 +2959,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -3308,7 +3305,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K15" s="64" t="s">
         <v>203</v>
@@ -3318,13 +3315,13 @@
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="236.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
-      <c r="B16" s="62" t="s">
-        <v>204</v>
+      <c r="B16" s="62">
+        <v>99460160</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3353,10 +3350,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K16" s="68" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
@@ -3369,7 +3366,7 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3398,10 +3395,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="66" t="s">
+        <v>207</v>
+      </c>
+      <c r="K17" s="66" t="s">
         <v>209</v>
-      </c>
-      <c r="K17" s="66" t="s">
-        <v>211</v>
       </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
@@ -3414,7 +3411,7 @@
         <v>IMG09</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3443,10 +3440,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K18" s="66" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
@@ -3488,7 +3485,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="67" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K19" s="68"/>
       <c r="O19" s="2" t="str">
@@ -3531,7 +3528,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="64" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K20" s="66"/>
       <c r="O20" s="2" t="str">
@@ -3574,7 +3571,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J21" s="66" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K21" s="66"/>
       <c r="O21" s="2" t="str">
@@ -3617,7 +3614,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="63" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K22" s="69"/>
       <c r="O22" s="2" t="str">

</xml_diff>